<commit_message>
Successfully displayed names according to quadrants!
</commit_message>
<xml_diff>
--- a/data/name_sheet_1_original.xlsx
+++ b/data/name_sheet_1_original.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Humbeads_interface\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1241E2DC-8512-4122-AC7C-2AF2B1CD7DE0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5800B92B-B364-40E7-9CCB-35224A5123E1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17932,9 +17932,6 @@
     <t>Doug Whitt</t>
   </si>
   <si>
-    <t>(illegible name starting with K between Doug Whitt and Martha Hess)</t>
-  </si>
-  <si>
     <t>Martha Hess</t>
   </si>
   <si>
@@ -18323,6 +18320,9 @@
   </si>
   <si>
     <t>Comedic; cinematic; television; radio</t>
+  </si>
+  <si>
+    <t>Kyle Creed</t>
   </si>
 </sst>
 </file>
@@ -18899,9 +18899,9 @@
   </sheetPr>
   <dimension ref="A1:AC1069"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A946" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E958" sqref="E958"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.26953125" defaultRowHeight="15" customHeight="1"/>
@@ -64396,7 +64396,7 @@
       <c r="A955" s="4"/>
       <c r="B955" s="5"/>
       <c r="C955" s="5" t="s">
-        <v>5194</v>
+        <v>5324</v>
       </c>
       <c r="D955" s="5"/>
       <c r="E955" s="5"/>
@@ -64431,7 +64431,7 @@
       <c r="A956" s="4"/>
       <c r="B956" s="5"/>
       <c r="C956" s="5" t="s">
-        <v>5195</v>
+        <v>5194</v>
       </c>
       <c r="D956" s="5"/>
       <c r="E956" s="5"/>
@@ -64466,7 +64466,7 @@
       <c r="A957" s="4"/>
       <c r="B957" s="5"/>
       <c r="C957" s="5" t="s">
-        <v>5196</v>
+        <v>5195</v>
       </c>
       <c r="D957" s="5"/>
       <c r="E957" s="5"/>
@@ -64501,7 +64501,7 @@
       <c r="A958" s="4"/>
       <c r="B958" s="5"/>
       <c r="C958" s="5" t="s">
-        <v>5197</v>
+        <v>5196</v>
       </c>
       <c r="D958" s="5"/>
       <c r="E958" s="5"/>
@@ -64536,7 +64536,7 @@
       <c r="A959" s="4"/>
       <c r="B959" s="5"/>
       <c r="C959" s="5" t="s">
-        <v>5198</v>
+        <v>5197</v>
       </c>
       <c r="D959" s="5"/>
       <c r="E959" s="5"/>
@@ -64571,7 +64571,7 @@
       <c r="A960" s="4"/>
       <c r="B960" s="5"/>
       <c r="C960" s="5" t="s">
-        <v>5199</v>
+        <v>5198</v>
       </c>
       <c r="D960" s="5"/>
       <c r="E960" s="5"/>
@@ -64606,7 +64606,7 @@
       <c r="A961" s="4"/>
       <c r="B961" s="5"/>
       <c r="C961" s="5" t="s">
-        <v>5200</v>
+        <v>5199</v>
       </c>
       <c r="D961" s="5"/>
       <c r="E961" s="5"/>
@@ -64641,7 +64641,7 @@
       <c r="A962" s="4"/>
       <c r="B962" s="5"/>
       <c r="C962" s="5" t="s">
-        <v>5201</v>
+        <v>5200</v>
       </c>
       <c r="D962" s="5"/>
       <c r="E962" s="5"/>
@@ -64676,7 +64676,7 @@
       <c r="A963" s="4"/>
       <c r="B963" s="5"/>
       <c r="C963" s="5" t="s">
-        <v>5202</v>
+        <v>5201</v>
       </c>
       <c r="D963" s="5"/>
       <c r="E963" s="5"/>
@@ -64711,7 +64711,7 @@
       <c r="A964" s="4"/>
       <c r="B964" s="5"/>
       <c r="C964" s="5" t="s">
-        <v>5203</v>
+        <v>5202</v>
       </c>
       <c r="D964" s="5"/>
       <c r="E964" s="5"/>
@@ -64746,7 +64746,7 @@
       <c r="A965" s="4"/>
       <c r="B965" s="5"/>
       <c r="C965" s="5" t="s">
-        <v>5204</v>
+        <v>5203</v>
       </c>
       <c r="D965" s="5"/>
       <c r="E965" s="5"/>
@@ -64781,7 +64781,7 @@
       <c r="A966" s="4"/>
       <c r="B966" s="5"/>
       <c r="C966" s="5" t="s">
-        <v>5205</v>
+        <v>5204</v>
       </c>
       <c r="D966" s="5"/>
       <c r="E966" s="5"/>
@@ -64816,7 +64816,7 @@
       <c r="A967" s="4"/>
       <c r="B967" s="5"/>
       <c r="C967" s="5" t="s">
-        <v>5206</v>
+        <v>5205</v>
       </c>
       <c r="D967" s="5"/>
       <c r="E967" s="5"/>
@@ -64886,7 +64886,7 @@
       <c r="A969" s="4"/>
       <c r="B969" s="5"/>
       <c r="C969" s="5" t="s">
-        <v>5207</v>
+        <v>5206</v>
       </c>
       <c r="D969" s="5"/>
       <c r="E969" s="5"/>
@@ -64921,7 +64921,7 @@
       <c r="A970" s="4"/>
       <c r="B970" s="5"/>
       <c r="C970" s="5" t="s">
-        <v>5208</v>
+        <v>5207</v>
       </c>
       <c r="D970" s="5"/>
       <c r="E970" s="5"/>
@@ -64936,7 +64936,7 @@
       <c r="N970" s="5"/>
       <c r="O970" s="5"/>
       <c r="P970" s="10" t="s">
-        <v>5209</v>
+        <v>5208</v>
       </c>
       <c r="Q970" s="5"/>
       <c r="R970" s="5"/>
@@ -64956,7 +64956,7 @@
       <c r="A971" s="4"/>
       <c r="B971" s="5"/>
       <c r="C971" s="5" t="s">
-        <v>5210</v>
+        <v>5209</v>
       </c>
       <c r="D971" s="5"/>
       <c r="E971" s="5"/>
@@ -64971,7 +64971,7 @@
       <c r="N971" s="5"/>
       <c r="O971" s="5"/>
       <c r="P971" s="10" t="s">
-        <v>5209</v>
+        <v>5208</v>
       </c>
       <c r="Q971" s="5"/>
       <c r="R971" s="5"/>
@@ -64991,7 +64991,7 @@
       <c r="A972" s="4"/>
       <c r="B972" s="5"/>
       <c r="C972" s="5" t="s">
-        <v>5211</v>
+        <v>5210</v>
       </c>
       <c r="D972" s="5"/>
       <c r="E972" s="5"/>
@@ -65006,7 +65006,7 @@
       <c r="N972" s="5"/>
       <c r="O972" s="5"/>
       <c r="P972" s="5" t="s">
-        <v>5209</v>
+        <v>5208</v>
       </c>
       <c r="Q972" s="5"/>
       <c r="R972" s="5"/>
@@ -65026,7 +65026,7 @@
       <c r="A973" s="4"/>
       <c r="B973" s="5"/>
       <c r="C973" s="5" t="s">
-        <v>5212</v>
+        <v>5211</v>
       </c>
       <c r="D973" s="5"/>
       <c r="E973" s="5"/>
@@ -65041,7 +65041,7 @@
       <c r="N973" s="5"/>
       <c r="O973" s="5"/>
       <c r="P973" s="5" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q973" s="5"/>
       <c r="R973" s="5"/>
@@ -65061,7 +65061,7 @@
       <c r="A974" s="4"/>
       <c r="B974" s="5"/>
       <c r="C974" s="5" t="s">
-        <v>5214</v>
+        <v>5213</v>
       </c>
       <c r="D974" s="5"/>
       <c r="E974" s="5"/>
@@ -65076,7 +65076,7 @@
       <c r="N974" s="5"/>
       <c r="O974" s="5"/>
       <c r="P974" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q974" s="5"/>
       <c r="R974" s="5"/>
@@ -65096,7 +65096,7 @@
       <c r="A975" s="4"/>
       <c r="B975" s="5"/>
       <c r="C975" s="5" t="s">
-        <v>5215</v>
+        <v>5214</v>
       </c>
       <c r="D975" s="5"/>
       <c r="E975" s="5"/>
@@ -65111,7 +65111,7 @@
       <c r="N975" s="5"/>
       <c r="O975" s="5"/>
       <c r="P975" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q975" s="5"/>
       <c r="R975" s="5"/>
@@ -65131,7 +65131,7 @@
       <c r="A976" s="4"/>
       <c r="B976" s="5"/>
       <c r="C976" s="5" t="s">
-        <v>5216</v>
+        <v>5215</v>
       </c>
       <c r="D976" s="5"/>
       <c r="E976" s="5"/>
@@ -65146,7 +65146,7 @@
       <c r="N976" s="5"/>
       <c r="O976" s="5"/>
       <c r="P976" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q976" s="5"/>
       <c r="R976" s="5"/>
@@ -65166,7 +65166,7 @@
       <c r="A977" s="4"/>
       <c r="B977" s="5"/>
       <c r="C977" s="5" t="s">
-        <v>5217</v>
+        <v>5216</v>
       </c>
       <c r="D977" s="5"/>
       <c r="E977" s="5"/>
@@ -65181,7 +65181,7 @@
       <c r="N977" s="5"/>
       <c r="O977" s="5"/>
       <c r="P977" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q977" s="5"/>
       <c r="R977" s="5"/>
@@ -65201,7 +65201,7 @@
       <c r="A978" s="4"/>
       <c r="B978" s="5"/>
       <c r="C978" s="5" t="s">
-        <v>5218</v>
+        <v>5217</v>
       </c>
       <c r="D978" s="5"/>
       <c r="E978" s="5"/>
@@ -65216,7 +65216,7 @@
       <c r="N978" s="5"/>
       <c r="O978" s="5"/>
       <c r="P978" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q978" s="5"/>
       <c r="R978" s="5"/>
@@ -65236,7 +65236,7 @@
       <c r="A979" s="4"/>
       <c r="B979" s="5"/>
       <c r="C979" s="5" t="s">
-        <v>5219</v>
+        <v>5218</v>
       </c>
       <c r="D979" s="5"/>
       <c r="E979" s="5"/>
@@ -65251,7 +65251,7 @@
       <c r="N979" s="5"/>
       <c r="O979" s="5"/>
       <c r="P979" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q979" s="5"/>
       <c r="R979" s="5"/>
@@ -65271,7 +65271,7 @@
       <c r="A980" s="4"/>
       <c r="B980" s="5"/>
       <c r="C980" s="5" t="s">
-        <v>5220</v>
+        <v>5219</v>
       </c>
       <c r="D980" s="5"/>
       <c r="E980" s="5"/>
@@ -65286,7 +65286,7 @@
       <c r="N980" s="5"/>
       <c r="O980" s="5"/>
       <c r="P980" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q980" s="5"/>
       <c r="R980" s="5"/>
@@ -65306,7 +65306,7 @@
       <c r="A981" s="4"/>
       <c r="B981" s="5"/>
       <c r="C981" s="5" t="s">
-        <v>5221</v>
+        <v>5220</v>
       </c>
       <c r="D981" s="5"/>
       <c r="E981" s="5"/>
@@ -65321,7 +65321,7 @@
       <c r="N981" s="5"/>
       <c r="O981" s="5"/>
       <c r="P981" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q981" s="5"/>
       <c r="R981" s="5"/>
@@ -65341,7 +65341,7 @@
       <c r="A982" s="4"/>
       <c r="B982" s="5"/>
       <c r="C982" s="5" t="s">
-        <v>5222</v>
+        <v>5221</v>
       </c>
       <c r="D982" s="5"/>
       <c r="E982" s="5"/>
@@ -65356,7 +65356,7 @@
       <c r="N982" s="5"/>
       <c r="O982" s="5"/>
       <c r="P982" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q982" s="5"/>
       <c r="R982" s="5"/>
@@ -65376,7 +65376,7 @@
       <c r="A983" s="4"/>
       <c r="B983" s="5"/>
       <c r="C983" s="5" t="s">
-        <v>5223</v>
+        <v>5222</v>
       </c>
       <c r="D983" s="5"/>
       <c r="E983" s="5"/>
@@ -65391,7 +65391,7 @@
       <c r="N983" s="5"/>
       <c r="O983" s="5"/>
       <c r="P983" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q983" s="5"/>
       <c r="R983" s="5"/>
@@ -65411,7 +65411,7 @@
       <c r="A984" s="4"/>
       <c r="B984" s="5"/>
       <c r="C984" s="5" t="s">
-        <v>5224</v>
+        <v>5223</v>
       </c>
       <c r="D984" s="5"/>
       <c r="E984" s="5"/>
@@ -65426,7 +65426,7 @@
       <c r="N984" s="5"/>
       <c r="O984" s="5"/>
       <c r="P984" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q984" s="5"/>
       <c r="R984" s="5"/>
@@ -65444,13 +65444,13 @@
     </row>
     <row r="985" spans="1:29">
       <c r="A985" s="4" t="s">
+        <v>5224</v>
+      </c>
+      <c r="B985" s="5" t="s">
         <v>5225</v>
       </c>
-      <c r="B985" s="5" t="s">
+      <c r="C985" s="5" t="s">
         <v>5226</v>
-      </c>
-      <c r="C985" s="5" t="s">
-        <v>5227</v>
       </c>
       <c r="D985" s="6">
         <v>4090</v>
@@ -65459,35 +65459,35 @@
         <v>31436</v>
       </c>
       <c r="F985" s="5" t="s">
+        <v>5227</v>
+      </c>
+      <c r="G985" s="5" t="s">
         <v>5228</v>
       </c>
-      <c r="G985" s="5" t="s">
+      <c r="H985" s="5" t="s">
         <v>5229</v>
       </c>
-      <c r="H985" s="5" t="s">
+      <c r="I985" s="9" t="s">
         <v>5230</v>
       </c>
-      <c r="I985" s="9" t="s">
+      <c r="J985" s="5" t="s">
         <v>5231</v>
       </c>
-      <c r="J985" s="5" t="s">
+      <c r="K985" s="11" t="s">
         <v>5232</v>
       </c>
-      <c r="K985" s="11" t="s">
+      <c r="L985" s="11" t="s">
         <v>5233</v>
-      </c>
-      <c r="L985" s="11" t="s">
-        <v>5234</v>
       </c>
       <c r="M985" s="5"/>
       <c r="N985" s="11" t="s">
+        <v>5234</v>
+      </c>
+      <c r="O985" s="5" t="s">
         <v>5235</v>
       </c>
-      <c r="O985" s="5" t="s">
-        <v>5236</v>
-      </c>
       <c r="P985" s="5" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q985" s="5"/>
       <c r="R985" s="5"/>
@@ -65507,7 +65507,7 @@
       <c r="A986" s="4"/>
       <c r="B986" s="5"/>
       <c r="C986" s="5" t="s">
-        <v>5237</v>
+        <v>5236</v>
       </c>
       <c r="D986" s="5"/>
       <c r="E986" s="5"/>
@@ -65522,7 +65522,7 @@
       <c r="N986" s="5"/>
       <c r="O986" s="5"/>
       <c r="P986" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q986" s="5"/>
       <c r="R986" s="5"/>
@@ -65542,7 +65542,7 @@
       <c r="A987" s="4"/>
       <c r="B987" s="5"/>
       <c r="C987" s="5" t="s">
-        <v>5238</v>
+        <v>5237</v>
       </c>
       <c r="D987" s="5"/>
       <c r="E987" s="5"/>
@@ -65557,7 +65557,7 @@
       <c r="N987" s="5"/>
       <c r="O987" s="5"/>
       <c r="P987" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q987" s="5"/>
       <c r="R987" s="5"/>
@@ -65577,7 +65577,7 @@
       <c r="A988" s="4"/>
       <c r="B988" s="5"/>
       <c r="C988" s="36" t="s">
-        <v>5239</v>
+        <v>5238</v>
       </c>
       <c r="D988" s="5"/>
       <c r="E988" s="5"/>
@@ -65592,7 +65592,7 @@
       <c r="N988" s="5"/>
       <c r="O988" s="5"/>
       <c r="P988" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q988" s="5"/>
       <c r="R988" s="5"/>
@@ -65612,7 +65612,7 @@
       <c r="A989" s="4"/>
       <c r="B989" s="5"/>
       <c r="C989" s="5" t="s">
-        <v>5240</v>
+        <v>5239</v>
       </c>
       <c r="D989" s="5"/>
       <c r="E989" s="5"/>
@@ -65627,7 +65627,7 @@
       <c r="N989" s="5"/>
       <c r="O989" s="5"/>
       <c r="P989" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q989" s="5"/>
       <c r="R989" s="5"/>
@@ -65647,7 +65647,7 @@
       <c r="A990" s="4"/>
       <c r="B990" s="5"/>
       <c r="C990" s="5" t="s">
-        <v>5241</v>
+        <v>5240</v>
       </c>
       <c r="D990" s="5"/>
       <c r="E990" s="5"/>
@@ -65662,7 +65662,7 @@
       <c r="N990" s="5"/>
       <c r="O990" s="5"/>
       <c r="P990" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q990" s="5"/>
       <c r="R990" s="5"/>
@@ -65682,7 +65682,7 @@
       <c r="A991" s="4"/>
       <c r="B991" s="5"/>
       <c r="C991" s="5" t="s">
-        <v>5242</v>
+        <v>5241</v>
       </c>
       <c r="D991" s="5"/>
       <c r="E991" s="5"/>
@@ -65697,7 +65697,7 @@
       <c r="N991" s="5"/>
       <c r="O991" s="5"/>
       <c r="P991" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q991" s="5"/>
       <c r="R991" s="5"/>
@@ -65717,7 +65717,7 @@
       <c r="A992" s="4"/>
       <c r="B992" s="5"/>
       <c r="C992" s="5" t="s">
-        <v>5243</v>
+        <v>5242</v>
       </c>
       <c r="D992" s="5"/>
       <c r="E992" s="5"/>
@@ -65732,7 +65732,7 @@
       <c r="N992" s="5"/>
       <c r="O992" s="5"/>
       <c r="P992" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q992" s="5"/>
       <c r="R992" s="5"/>
@@ -65752,7 +65752,7 @@
       <c r="A993" s="4"/>
       <c r="B993" s="5"/>
       <c r="C993" s="5" t="s">
-        <v>5244</v>
+        <v>5243</v>
       </c>
       <c r="D993" s="5"/>
       <c r="E993" s="5"/>
@@ -65767,7 +65767,7 @@
       <c r="N993" s="5"/>
       <c r="O993" s="5"/>
       <c r="P993" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q993" s="5"/>
       <c r="R993" s="5"/>
@@ -65787,7 +65787,7 @@
       <c r="A994" s="4"/>
       <c r="B994" s="5"/>
       <c r="C994" s="5" t="s">
-        <v>5245</v>
+        <v>5244</v>
       </c>
       <c r="D994" s="5"/>
       <c r="E994" s="5"/>
@@ -65802,7 +65802,7 @@
       <c r="N994" s="5"/>
       <c r="O994" s="5"/>
       <c r="P994" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q994" s="5"/>
       <c r="R994" s="5"/>
@@ -65822,7 +65822,7 @@
       <c r="A995" s="4"/>
       <c r="B995" s="5"/>
       <c r="C995" s="5" t="s">
-        <v>5246</v>
+        <v>5245</v>
       </c>
       <c r="D995" s="5"/>
       <c r="E995" s="5"/>
@@ -65837,7 +65837,7 @@
       <c r="N995" s="5"/>
       <c r="O995" s="5"/>
       <c r="P995" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q995" s="5"/>
       <c r="R995" s="5"/>
@@ -65857,7 +65857,7 @@
       <c r="A996" s="4"/>
       <c r="B996" s="5"/>
       <c r="C996" s="5" t="s">
-        <v>5247</v>
+        <v>5246</v>
       </c>
       <c r="D996" s="5"/>
       <c r="E996" s="5"/>
@@ -65872,7 +65872,7 @@
       <c r="N996" s="5"/>
       <c r="O996" s="5"/>
       <c r="P996" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q996" s="5"/>
       <c r="R996" s="5"/>
@@ -65892,7 +65892,7 @@
       <c r="A997" s="4"/>
       <c r="B997" s="5"/>
       <c r="C997" s="5" t="s">
-        <v>5248</v>
+        <v>5247</v>
       </c>
       <c r="D997" s="5"/>
       <c r="E997" s="5"/>
@@ -65907,7 +65907,7 @@
       <c r="N997" s="5"/>
       <c r="O997" s="5"/>
       <c r="P997" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q997" s="5"/>
       <c r="R997" s="5"/>
@@ -65927,7 +65927,7 @@
       <c r="A998" s="4"/>
       <c r="B998" s="5"/>
       <c r="C998" s="5" t="s">
-        <v>5249</v>
+        <v>5248</v>
       </c>
       <c r="D998" s="5"/>
       <c r="E998" s="5"/>
@@ -65942,7 +65942,7 @@
       <c r="N998" s="5"/>
       <c r="O998" s="5"/>
       <c r="P998" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q998" s="5"/>
       <c r="R998" s="5"/>
@@ -65962,7 +65962,7 @@
       <c r="A999" s="4"/>
       <c r="B999" s="5"/>
       <c r="C999" s="36" t="s">
-        <v>5250</v>
+        <v>5249</v>
       </c>
       <c r="D999" s="5"/>
       <c r="E999" s="5"/>
@@ -65977,7 +65977,7 @@
       <c r="N999" s="5"/>
       <c r="O999" s="5"/>
       <c r="P999" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q999" s="5"/>
       <c r="R999" s="5"/>
@@ -65997,7 +65997,7 @@
       <c r="A1000" s="4"/>
       <c r="B1000" s="5"/>
       <c r="C1000" s="5" t="s">
-        <v>5251</v>
+        <v>5250</v>
       </c>
       <c r="D1000" s="5"/>
       <c r="E1000" s="5"/>
@@ -66012,7 +66012,7 @@
       <c r="N1000" s="5"/>
       <c r="O1000" s="5"/>
       <c r="P1000" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q1000" s="5"/>
       <c r="R1000" s="5"/>
@@ -66032,7 +66032,7 @@
       <c r="A1001" s="4"/>
       <c r="B1001" s="5"/>
       <c r="C1001" s="5" t="s">
-        <v>5252</v>
+        <v>5251</v>
       </c>
       <c r="D1001" s="5"/>
       <c r="E1001" s="5"/>
@@ -66047,7 +66047,7 @@
       <c r="N1001" s="5"/>
       <c r="O1001" s="5"/>
       <c r="P1001" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q1001" s="5"/>
       <c r="R1001" s="5"/>
@@ -66067,7 +66067,7 @@
       <c r="A1002" s="4"/>
       <c r="B1002" s="5"/>
       <c r="C1002" s="5" t="s">
-        <v>5253</v>
+        <v>5252</v>
       </c>
       <c r="D1002" s="5"/>
       <c r="E1002" s="5"/>
@@ -66082,7 +66082,7 @@
       <c r="N1002" s="5"/>
       <c r="O1002" s="5"/>
       <c r="P1002" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q1002" s="5"/>
       <c r="R1002" s="5"/>
@@ -66102,7 +66102,7 @@
       <c r="A1003" s="4"/>
       <c r="B1003" s="5"/>
       <c r="C1003" s="5" t="s">
-        <v>5254</v>
+        <v>5253</v>
       </c>
       <c r="D1003" s="5"/>
       <c r="E1003" s="5"/>
@@ -66117,7 +66117,7 @@
       <c r="N1003" s="5"/>
       <c r="O1003" s="5"/>
       <c r="P1003" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q1003" s="5"/>
       <c r="R1003" s="5"/>
@@ -66137,7 +66137,7 @@
       <c r="A1004" s="4"/>
       <c r="B1004" s="5"/>
       <c r="C1004" s="5" t="s">
-        <v>5255</v>
+        <v>5254</v>
       </c>
       <c r="D1004" s="5"/>
       <c r="E1004" s="5"/>
@@ -66152,7 +66152,7 @@
       <c r="N1004" s="5"/>
       <c r="O1004" s="5"/>
       <c r="P1004" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q1004" s="5"/>
       <c r="R1004" s="5"/>
@@ -66172,7 +66172,7 @@
       <c r="A1005" s="4"/>
       <c r="B1005" s="5"/>
       <c r="C1005" s="5" t="s">
-        <v>5256</v>
+        <v>5255</v>
       </c>
       <c r="D1005" s="5"/>
       <c r="E1005" s="5"/>
@@ -66187,7 +66187,7 @@
       <c r="N1005" s="5"/>
       <c r="O1005" s="5"/>
       <c r="P1005" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q1005" s="5"/>
       <c r="R1005" s="5"/>
@@ -66207,7 +66207,7 @@
       <c r="A1006" s="4"/>
       <c r="B1006" s="5"/>
       <c r="C1006" s="5" t="s">
-        <v>5257</v>
+        <v>5256</v>
       </c>
       <c r="D1006" s="5"/>
       <c r="E1006" s="5"/>
@@ -66222,7 +66222,7 @@
       <c r="N1006" s="5"/>
       <c r="O1006" s="5"/>
       <c r="P1006" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q1006" s="5"/>
       <c r="R1006" s="5"/>
@@ -66242,7 +66242,7 @@
       <c r="A1007" s="4"/>
       <c r="B1007" s="5"/>
       <c r="C1007" s="5" t="s">
-        <v>5258</v>
+        <v>5257</v>
       </c>
       <c r="D1007" s="5"/>
       <c r="E1007" s="5"/>
@@ -66257,7 +66257,7 @@
       <c r="N1007" s="5"/>
       <c r="O1007" s="5"/>
       <c r="P1007" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q1007" s="5"/>
       <c r="R1007" s="5"/>
@@ -66292,7 +66292,7 @@
       <c r="N1008" s="5"/>
       <c r="O1008" s="5"/>
       <c r="P1008" s="10" t="s">
-        <v>5213</v>
+        <v>5212</v>
       </c>
       <c r="Q1008" s="5"/>
       <c r="R1008" s="5"/>
@@ -66312,7 +66312,7 @@
       <c r="A1009" s="4"/>
       <c r="B1009" s="5"/>
       <c r="C1009" s="5" t="s">
-        <v>5259</v>
+        <v>5258</v>
       </c>
       <c r="D1009" s="5"/>
       <c r="E1009" s="5"/>
@@ -66327,7 +66327,7 @@
       <c r="N1009" s="5"/>
       <c r="O1009" s="5"/>
       <c r="P1009" s="10" t="s">
-        <v>5260</v>
+        <v>5259</v>
       </c>
       <c r="Q1009" s="5"/>
       <c r="R1009" s="5"/>
@@ -66347,7 +66347,7 @@
       <c r="A1010" s="4"/>
       <c r="B1010" s="5"/>
       <c r="C1010" s="5" t="s">
-        <v>5261</v>
+        <v>5260</v>
       </c>
       <c r="D1010" s="5"/>
       <c r="E1010" s="5"/>
@@ -66362,7 +66362,7 @@
       <c r="N1010" s="5"/>
       <c r="O1010" s="5"/>
       <c r="P1010" s="10" t="s">
-        <v>5260</v>
+        <v>5259</v>
       </c>
       <c r="Q1010" s="5"/>
       <c r="R1010" s="5"/>
@@ -66382,7 +66382,7 @@
       <c r="A1011" s="4"/>
       <c r="B1011" s="5"/>
       <c r="C1011" s="5" t="s">
-        <v>5262</v>
+        <v>5261</v>
       </c>
       <c r="D1011" s="5"/>
       <c r="E1011" s="5"/>
@@ -66397,7 +66397,7 @@
       <c r="N1011" s="5"/>
       <c r="O1011" s="5"/>
       <c r="P1011" s="10" t="s">
-        <v>5260</v>
+        <v>5259</v>
       </c>
       <c r="Q1011" s="5"/>
       <c r="R1011" s="5"/>
@@ -66417,7 +66417,7 @@
       <c r="A1012" s="4"/>
       <c r="B1012" s="5"/>
       <c r="C1012" s="5" t="s">
-        <v>5263</v>
+        <v>5262</v>
       </c>
       <c r="D1012" s="5"/>
       <c r="E1012" s="5"/>
@@ -66432,7 +66432,7 @@
       <c r="N1012" s="5"/>
       <c r="O1012" s="5"/>
       <c r="P1012" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1012" s="5"/>
       <c r="R1012" s="5"/>
@@ -66452,7 +66452,7 @@
       <c r="A1013" s="4"/>
       <c r="B1013" s="5"/>
       <c r="C1013" s="5" t="s">
-        <v>5265</v>
+        <v>5264</v>
       </c>
       <c r="D1013" s="5"/>
       <c r="E1013" s="5"/>
@@ -66467,12 +66467,12 @@
       <c r="N1013" s="5"/>
       <c r="O1013" s="5"/>
       <c r="P1013" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1013" s="5"/>
       <c r="R1013" s="5"/>
       <c r="S1013" s="4" t="s">
-        <v>5266</v>
+        <v>5265</v>
       </c>
       <c r="T1013" s="3"/>
       <c r="U1013" s="3"/>
@@ -66489,7 +66489,7 @@
       <c r="A1014" s="4"/>
       <c r="B1014" s="5"/>
       <c r="C1014" s="5" t="s">
-        <v>5267</v>
+        <v>5266</v>
       </c>
       <c r="D1014" s="5"/>
       <c r="E1014" s="5"/>
@@ -66504,7 +66504,7 @@
       <c r="N1014" s="5"/>
       <c r="O1014" s="5"/>
       <c r="P1014" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1014" s="5"/>
       <c r="R1014" s="5"/>
@@ -66524,7 +66524,7 @@
       <c r="A1015" s="4"/>
       <c r="B1015" s="5"/>
       <c r="C1015" s="36" t="s">
-        <v>5268</v>
+        <v>5267</v>
       </c>
       <c r="D1015" s="5"/>
       <c r="E1015" s="5"/>
@@ -66539,7 +66539,7 @@
       <c r="N1015" s="5"/>
       <c r="O1015" s="5"/>
       <c r="P1015" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1015" s="5"/>
       <c r="R1015" s="5"/>
@@ -66559,7 +66559,7 @@
       <c r="A1016" s="4"/>
       <c r="B1016" s="5"/>
       <c r="C1016" s="5" t="s">
-        <v>5269</v>
+        <v>5268</v>
       </c>
       <c r="D1016" s="5"/>
       <c r="E1016" s="5"/>
@@ -66574,7 +66574,7 @@
       <c r="N1016" s="5"/>
       <c r="O1016" s="5"/>
       <c r="P1016" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1016" s="5"/>
       <c r="R1016" s="5"/>
@@ -66594,7 +66594,7 @@
       <c r="A1017" s="4"/>
       <c r="B1017" s="5"/>
       <c r="C1017" s="36" t="s">
-        <v>5270</v>
+        <v>5269</v>
       </c>
       <c r="D1017" s="5"/>
       <c r="E1017" s="5"/>
@@ -66609,7 +66609,7 @@
       <c r="N1017" s="5"/>
       <c r="O1017" s="5"/>
       <c r="P1017" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1017" s="5"/>
       <c r="R1017" s="5"/>
@@ -66629,7 +66629,7 @@
       <c r="A1018" s="4"/>
       <c r="B1018" s="5"/>
       <c r="C1018" s="5" t="s">
-        <v>5271</v>
+        <v>5270</v>
       </c>
       <c r="D1018" s="5"/>
       <c r="E1018" s="5"/>
@@ -66644,7 +66644,7 @@
       <c r="N1018" s="5"/>
       <c r="O1018" s="5"/>
       <c r="P1018" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1018" s="5"/>
       <c r="R1018" s="5"/>
@@ -66664,7 +66664,7 @@
       <c r="A1019" s="4"/>
       <c r="B1019" s="5"/>
       <c r="C1019" s="5" t="s">
-        <v>5272</v>
+        <v>5271</v>
       </c>
       <c r="D1019" s="5"/>
       <c r="E1019" s="5"/>
@@ -66679,7 +66679,7 @@
       <c r="N1019" s="5"/>
       <c r="O1019" s="5"/>
       <c r="P1019" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1019" s="5"/>
       <c r="R1019" s="5"/>
@@ -66699,7 +66699,7 @@
       <c r="A1020" s="4"/>
       <c r="B1020" s="5"/>
       <c r="C1020" s="36" t="s">
-        <v>5273</v>
+        <v>5272</v>
       </c>
       <c r="D1020" s="5"/>
       <c r="E1020" s="5"/>
@@ -66714,7 +66714,7 @@
       <c r="N1020" s="5"/>
       <c r="O1020" s="5"/>
       <c r="P1020" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1020" s="5"/>
       <c r="R1020" s="5"/>
@@ -66734,7 +66734,7 @@
       <c r="A1021" s="4"/>
       <c r="B1021" s="5"/>
       <c r="C1021" s="5" t="s">
-        <v>5274</v>
+        <v>5273</v>
       </c>
       <c r="D1021" s="5"/>
       <c r="E1021" s="5"/>
@@ -66749,7 +66749,7 @@
       <c r="N1021" s="5"/>
       <c r="O1021" s="5"/>
       <c r="P1021" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1021" s="5"/>
       <c r="R1021" s="5"/>
@@ -66769,7 +66769,7 @@
       <c r="A1022" s="4"/>
       <c r="B1022" s="5"/>
       <c r="C1022" s="5" t="s">
-        <v>5275</v>
+        <v>5274</v>
       </c>
       <c r="D1022" s="5"/>
       <c r="E1022" s="5"/>
@@ -66784,7 +66784,7 @@
       <c r="N1022" s="5"/>
       <c r="O1022" s="5"/>
       <c r="P1022" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1022" s="5"/>
       <c r="R1022" s="5"/>
@@ -66804,7 +66804,7 @@
       <c r="A1023" s="4"/>
       <c r="B1023" s="5"/>
       <c r="C1023" s="5" t="s">
-        <v>5276</v>
+        <v>5275</v>
       </c>
       <c r="D1023" s="5"/>
       <c r="E1023" s="5"/>
@@ -66819,7 +66819,7 @@
       <c r="N1023" s="5"/>
       <c r="O1023" s="5"/>
       <c r="P1023" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1023" s="5"/>
       <c r="R1023" s="5"/>
@@ -66839,7 +66839,7 @@
       <c r="A1024" s="4"/>
       <c r="B1024" s="5"/>
       <c r="C1024" s="5" t="s">
-        <v>5277</v>
+        <v>5276</v>
       </c>
       <c r="D1024" s="5"/>
       <c r="E1024" s="5"/>
@@ -66854,7 +66854,7 @@
       <c r="N1024" s="5"/>
       <c r="O1024" s="5"/>
       <c r="P1024" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1024" s="5"/>
       <c r="R1024" s="5"/>
@@ -66874,7 +66874,7 @@
       <c r="A1025" s="4"/>
       <c r="B1025" s="5"/>
       <c r="C1025" s="5" t="s">
-        <v>5278</v>
+        <v>5277</v>
       </c>
       <c r="D1025" s="5"/>
       <c r="E1025" s="5"/>
@@ -66889,7 +66889,7 @@
       <c r="N1025" s="5"/>
       <c r="O1025" s="5"/>
       <c r="P1025" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1025" s="5"/>
       <c r="R1025" s="5"/>
@@ -66909,7 +66909,7 @@
       <c r="A1026" s="4"/>
       <c r="B1026" s="5"/>
       <c r="C1026" s="5" t="s">
-        <v>5279</v>
+        <v>5278</v>
       </c>
       <c r="D1026" s="5"/>
       <c r="E1026" s="5"/>
@@ -66924,7 +66924,7 @@
       <c r="N1026" s="5"/>
       <c r="O1026" s="5"/>
       <c r="P1026" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1026" s="5"/>
       <c r="R1026" s="5"/>
@@ -66944,7 +66944,7 @@
       <c r="A1027" s="4"/>
       <c r="B1027" s="5"/>
       <c r="C1027" s="8" t="s">
-        <v>5280</v>
+        <v>5279</v>
       </c>
       <c r="D1027" s="5"/>
       <c r="E1027" s="5"/>
@@ -66959,7 +66959,7 @@
       <c r="N1027" s="5"/>
       <c r="O1027" s="5"/>
       <c r="P1027" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1027" s="5"/>
       <c r="R1027" s="5"/>
@@ -66979,7 +66979,7 @@
       <c r="A1028" s="4"/>
       <c r="B1028" s="5"/>
       <c r="C1028" s="5" t="s">
-        <v>5281</v>
+        <v>5280</v>
       </c>
       <c r="D1028" s="5"/>
       <c r="E1028" s="5"/>
@@ -66994,7 +66994,7 @@
       <c r="N1028" s="5"/>
       <c r="O1028" s="5"/>
       <c r="P1028" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1028" s="5"/>
       <c r="R1028" s="5"/>
@@ -67014,7 +67014,7 @@
       <c r="A1029" s="4"/>
       <c r="B1029" s="5"/>
       <c r="C1029" s="5" t="s">
-        <v>5282</v>
+        <v>5281</v>
       </c>
       <c r="D1029" s="5"/>
       <c r="E1029" s="5"/>
@@ -67029,7 +67029,7 @@
       <c r="N1029" s="5"/>
       <c r="O1029" s="5"/>
       <c r="P1029" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1029" s="5"/>
       <c r="R1029" s="5"/>
@@ -67049,7 +67049,7 @@
       <c r="A1030" s="4"/>
       <c r="B1030" s="5"/>
       <c r="C1030" s="5" t="s">
-        <v>5283</v>
+        <v>5282</v>
       </c>
       <c r="D1030" s="5"/>
       <c r="E1030" s="5"/>
@@ -67064,7 +67064,7 @@
       <c r="N1030" s="5"/>
       <c r="O1030" s="5"/>
       <c r="P1030" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1030" s="5"/>
       <c r="R1030" s="5"/>
@@ -67084,7 +67084,7 @@
       <c r="A1031" s="4"/>
       <c r="B1031" s="5"/>
       <c r="C1031" s="5" t="s">
-        <v>5284</v>
+        <v>5283</v>
       </c>
       <c r="D1031" s="5"/>
       <c r="E1031" s="5"/>
@@ -67099,7 +67099,7 @@
       <c r="N1031" s="5"/>
       <c r="O1031" s="5"/>
       <c r="P1031" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1031" s="5"/>
       <c r="R1031" s="5"/>
@@ -67119,7 +67119,7 @@
       <c r="A1032" s="4"/>
       <c r="B1032" s="5"/>
       <c r="C1032" s="5" t="s">
-        <v>5285</v>
+        <v>5284</v>
       </c>
       <c r="D1032" s="5"/>
       <c r="E1032" s="5"/>
@@ -67134,7 +67134,7 @@
       <c r="N1032" s="5"/>
       <c r="O1032" s="5"/>
       <c r="P1032" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1032" s="5"/>
       <c r="R1032" s="5"/>
@@ -67154,7 +67154,7 @@
       <c r="A1033" s="4"/>
       <c r="B1033" s="5"/>
       <c r="C1033" s="5" t="s">
-        <v>5286</v>
+        <v>5285</v>
       </c>
       <c r="D1033" s="5"/>
       <c r="E1033" s="5"/>
@@ -67169,7 +67169,7 @@
       <c r="N1033" s="5"/>
       <c r="O1033" s="5"/>
       <c r="P1033" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1033" s="5"/>
       <c r="R1033" s="5"/>
@@ -67189,7 +67189,7 @@
       <c r="A1034" s="4"/>
       <c r="B1034" s="5"/>
       <c r="C1034" s="5" t="s">
-        <v>5287</v>
+        <v>5286</v>
       </c>
       <c r="D1034" s="5"/>
       <c r="E1034" s="5"/>
@@ -67204,7 +67204,7 @@
       <c r="N1034" s="5"/>
       <c r="O1034" s="5"/>
       <c r="P1034" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1034" s="5"/>
       <c r="R1034" s="5"/>
@@ -67224,7 +67224,7 @@
       <c r="A1035" s="4"/>
       <c r="B1035" s="5"/>
       <c r="C1035" s="5" t="s">
-        <v>5288</v>
+        <v>5287</v>
       </c>
       <c r="D1035" s="5"/>
       <c r="E1035" s="5"/>
@@ -67239,7 +67239,7 @@
       <c r="N1035" s="5"/>
       <c r="O1035" s="5"/>
       <c r="P1035" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1035" s="5"/>
       <c r="R1035" s="5"/>
@@ -67259,7 +67259,7 @@
       <c r="A1036" s="4"/>
       <c r="B1036" s="5"/>
       <c r="C1036" s="5" t="s">
-        <v>5289</v>
+        <v>5288</v>
       </c>
       <c r="D1036" s="5"/>
       <c r="E1036" s="5"/>
@@ -67274,7 +67274,7 @@
       <c r="N1036" s="5"/>
       <c r="O1036" s="5"/>
       <c r="P1036" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1036" s="5"/>
       <c r="R1036" s="5"/>
@@ -67294,7 +67294,7 @@
       <c r="A1037" s="4"/>
       <c r="B1037" s="5"/>
       <c r="C1037" s="5" t="s">
-        <v>5290</v>
+        <v>5289</v>
       </c>
       <c r="D1037" s="5"/>
       <c r="E1037" s="5"/>
@@ -67309,7 +67309,7 @@
       <c r="N1037" s="5"/>
       <c r="O1037" s="5"/>
       <c r="P1037" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1037" s="5"/>
       <c r="R1037" s="5"/>
@@ -67329,7 +67329,7 @@
       <c r="A1038" s="4"/>
       <c r="B1038" s="5"/>
       <c r="C1038" s="5" t="s">
-        <v>5291</v>
+        <v>5290</v>
       </c>
       <c r="D1038" s="5"/>
       <c r="E1038" s="5"/>
@@ -67344,7 +67344,7 @@
       <c r="N1038" s="5"/>
       <c r="O1038" s="5"/>
       <c r="P1038" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1038" s="5"/>
       <c r="R1038" s="5"/>
@@ -67364,7 +67364,7 @@
       <c r="A1039" s="4"/>
       <c r="B1039" s="5"/>
       <c r="C1039" s="5" t="s">
-        <v>5292</v>
+        <v>5291</v>
       </c>
       <c r="D1039" s="5"/>
       <c r="E1039" s="5"/>
@@ -67379,7 +67379,7 @@
       <c r="N1039" s="5"/>
       <c r="O1039" s="5"/>
       <c r="P1039" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1039" s="5"/>
       <c r="R1039" s="5"/>
@@ -67399,7 +67399,7 @@
       <c r="A1040" s="4"/>
       <c r="B1040" s="5"/>
       <c r="C1040" s="5" t="s">
-        <v>5293</v>
+        <v>5292</v>
       </c>
       <c r="D1040" s="5"/>
       <c r="E1040" s="5"/>
@@ -67414,7 +67414,7 @@
       <c r="N1040" s="5"/>
       <c r="O1040" s="5"/>
       <c r="P1040" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1040" s="5"/>
       <c r="R1040" s="5"/>
@@ -67434,7 +67434,7 @@
       <c r="A1041" s="4"/>
       <c r="B1041" s="5"/>
       <c r="C1041" s="5" t="s">
-        <v>5294</v>
+        <v>5293</v>
       </c>
       <c r="D1041" s="5"/>
       <c r="E1041" s="5"/>
@@ -67449,7 +67449,7 @@
       <c r="N1041" s="5"/>
       <c r="O1041" s="5"/>
       <c r="P1041" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1041" s="5"/>
       <c r="R1041" s="5"/>
@@ -67469,7 +67469,7 @@
       <c r="A1042" s="4"/>
       <c r="B1042" s="5"/>
       <c r="C1042" s="5" t="s">
-        <v>5295</v>
+        <v>5294</v>
       </c>
       <c r="D1042" s="5"/>
       <c r="E1042" s="5"/>
@@ -67484,7 +67484,7 @@
       <c r="N1042" s="5"/>
       <c r="O1042" s="5"/>
       <c r="P1042" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1042" s="5"/>
       <c r="R1042" s="5"/>
@@ -67504,7 +67504,7 @@
       <c r="A1043" s="4"/>
       <c r="B1043" s="5"/>
       <c r="C1043" s="5" t="s">
-        <v>5296</v>
+        <v>5295</v>
       </c>
       <c r="D1043" s="5"/>
       <c r="E1043" s="5"/>
@@ -67519,7 +67519,7 @@
       <c r="N1043" s="5"/>
       <c r="O1043" s="5"/>
       <c r="P1043" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1043" s="5"/>
       <c r="R1043" s="5"/>
@@ -67539,7 +67539,7 @@
       <c r="A1044" s="4"/>
       <c r="B1044" s="5"/>
       <c r="C1044" s="5" t="s">
-        <v>5297</v>
+        <v>5296</v>
       </c>
       <c r="D1044" s="5"/>
       <c r="E1044" s="5"/>
@@ -67554,7 +67554,7 @@
       <c r="N1044" s="5"/>
       <c r="O1044" s="5"/>
       <c r="P1044" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1044" s="5"/>
       <c r="R1044" s="5"/>
@@ -67574,7 +67574,7 @@
       <c r="A1045" s="4"/>
       <c r="B1045" s="5"/>
       <c r="C1045" s="5" t="s">
-        <v>5298</v>
+        <v>5297</v>
       </c>
       <c r="D1045" s="5"/>
       <c r="E1045" s="5"/>
@@ -67589,7 +67589,7 @@
       <c r="N1045" s="5"/>
       <c r="O1045" s="5"/>
       <c r="P1045" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1045" s="5"/>
       <c r="R1045" s="5"/>
@@ -67609,7 +67609,7 @@
       <c r="A1046" s="4"/>
       <c r="B1046" s="5"/>
       <c r="C1046" s="5" t="s">
-        <v>5299</v>
+        <v>5298</v>
       </c>
       <c r="D1046" s="5"/>
       <c r="E1046" s="5"/>
@@ -67624,7 +67624,7 @@
       <c r="N1046" s="5"/>
       <c r="O1046" s="5"/>
       <c r="P1046" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1046" s="5"/>
       <c r="R1046" s="5"/>
@@ -67644,7 +67644,7 @@
       <c r="A1047" s="4"/>
       <c r="B1047" s="5"/>
       <c r="C1047" s="5" t="s">
-        <v>5300</v>
+        <v>5299</v>
       </c>
       <c r="D1047" s="5"/>
       <c r="E1047" s="5"/>
@@ -67659,7 +67659,7 @@
       <c r="N1047" s="5"/>
       <c r="O1047" s="5"/>
       <c r="P1047" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1047" s="5"/>
       <c r="R1047" s="5"/>
@@ -67679,7 +67679,7 @@
       <c r="A1048" s="4"/>
       <c r="B1048" s="5"/>
       <c r="C1048" s="5" t="s">
-        <v>5301</v>
+        <v>5300</v>
       </c>
       <c r="D1048" s="5"/>
       <c r="E1048" s="5"/>
@@ -67694,7 +67694,7 @@
       <c r="N1048" s="5"/>
       <c r="O1048" s="5"/>
       <c r="P1048" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1048" s="5"/>
       <c r="R1048" s="5"/>
@@ -67714,7 +67714,7 @@
       <c r="A1049" s="4"/>
       <c r="B1049" s="5"/>
       <c r="C1049" s="5" t="s">
-        <v>5302</v>
+        <v>5301</v>
       </c>
       <c r="D1049" s="5"/>
       <c r="E1049" s="5"/>
@@ -67729,7 +67729,7 @@
       <c r="N1049" s="5"/>
       <c r="O1049" s="5"/>
       <c r="P1049" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1049" s="5"/>
       <c r="R1049" s="5"/>
@@ -67749,7 +67749,7 @@
       <c r="A1050" s="4"/>
       <c r="B1050" s="5"/>
       <c r="C1050" s="5" t="s">
-        <v>5303</v>
+        <v>5302</v>
       </c>
       <c r="D1050" s="5"/>
       <c r="E1050" s="5"/>
@@ -67764,7 +67764,7 @@
       <c r="N1050" s="5"/>
       <c r="O1050" s="5"/>
       <c r="P1050" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1050" s="5"/>
       <c r="R1050" s="5"/>
@@ -67784,7 +67784,7 @@
       <c r="A1051" s="4"/>
       <c r="B1051" s="5"/>
       <c r="C1051" s="5" t="s">
-        <v>5304</v>
+        <v>5303</v>
       </c>
       <c r="D1051" s="5"/>
       <c r="E1051" s="5"/>
@@ -67799,7 +67799,7 @@
       <c r="N1051" s="5"/>
       <c r="O1051" s="5"/>
       <c r="P1051" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1051" s="5"/>
       <c r="R1051" s="5"/>
@@ -67819,7 +67819,7 @@
       <c r="A1052" s="4"/>
       <c r="B1052" s="5"/>
       <c r="C1052" s="5" t="s">
-        <v>5305</v>
+        <v>5304</v>
       </c>
       <c r="D1052" s="5"/>
       <c r="E1052" s="5"/>
@@ -67834,7 +67834,7 @@
       <c r="N1052" s="5"/>
       <c r="O1052" s="5"/>
       <c r="P1052" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1052" s="5"/>
       <c r="R1052" s="5"/>
@@ -67869,7 +67869,7 @@
       <c r="N1053" s="5"/>
       <c r="O1053" s="5"/>
       <c r="P1053" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1053" s="5"/>
       <c r="R1053" s="5"/>
@@ -67889,7 +67889,7 @@
       <c r="A1054" s="4"/>
       <c r="B1054" s="5"/>
       <c r="C1054" s="5" t="s">
-        <v>5306</v>
+        <v>5305</v>
       </c>
       <c r="D1054" s="5"/>
       <c r="E1054" s="5"/>
@@ -67904,7 +67904,7 @@
       <c r="N1054" s="5"/>
       <c r="O1054" s="5"/>
       <c r="P1054" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1054" s="5"/>
       <c r="R1054" s="5"/>
@@ -67924,7 +67924,7 @@
       <c r="A1055" s="4"/>
       <c r="B1055" s="5"/>
       <c r="C1055" s="5" t="s">
-        <v>5307</v>
+        <v>5306</v>
       </c>
       <c r="D1055" s="5"/>
       <c r="E1055" s="5"/>
@@ -67939,7 +67939,7 @@
       <c r="N1055" s="5"/>
       <c r="O1055" s="5"/>
       <c r="P1055" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1055" s="5"/>
       <c r="R1055" s="5"/>
@@ -67959,7 +67959,7 @@
       <c r="A1056" s="4"/>
       <c r="B1056" s="5"/>
       <c r="C1056" s="5" t="s">
-        <v>5308</v>
+        <v>5307</v>
       </c>
       <c r="D1056" s="5"/>
       <c r="E1056" s="5"/>
@@ -67974,7 +67974,7 @@
       <c r="N1056" s="5"/>
       <c r="O1056" s="5"/>
       <c r="P1056" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1056" s="5"/>
       <c r="R1056" s="5"/>
@@ -67994,7 +67994,7 @@
       <c r="A1057" s="4"/>
       <c r="B1057" s="5"/>
       <c r="C1057" s="5" t="s">
-        <v>5309</v>
+        <v>5308</v>
       </c>
       <c r="D1057" s="5"/>
       <c r="E1057" s="5"/>
@@ -68009,7 +68009,7 @@
       <c r="N1057" s="5"/>
       <c r="O1057" s="5"/>
       <c r="P1057" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1057" s="5"/>
       <c r="R1057" s="5"/>
@@ -68029,7 +68029,7 @@
       <c r="A1058" s="4"/>
       <c r="B1058" s="5"/>
       <c r="C1058" s="36" t="s">
-        <v>5310</v>
+        <v>5309</v>
       </c>
       <c r="D1058" s="5"/>
       <c r="E1058" s="5"/>
@@ -68044,7 +68044,7 @@
       <c r="N1058" s="5"/>
       <c r="O1058" s="5"/>
       <c r="P1058" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1058" s="5"/>
       <c r="R1058" s="5"/>
@@ -68064,7 +68064,7 @@
       <c r="A1059" s="4"/>
       <c r="B1059" s="5"/>
       <c r="C1059" s="5" t="s">
-        <v>5311</v>
+        <v>5310</v>
       </c>
       <c r="D1059" s="5"/>
       <c r="E1059" s="5"/>
@@ -68079,7 +68079,7 @@
       <c r="N1059" s="5"/>
       <c r="O1059" s="5"/>
       <c r="P1059" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1059" s="5"/>
       <c r="R1059" s="5"/>
@@ -68099,7 +68099,7 @@
       <c r="A1060" s="4"/>
       <c r="B1060" s="5"/>
       <c r="C1060" s="5" t="s">
-        <v>5312</v>
+        <v>5311</v>
       </c>
       <c r="D1060" s="5"/>
       <c r="E1060" s="5"/>
@@ -68114,7 +68114,7 @@
       <c r="N1060" s="5"/>
       <c r="O1060" s="5"/>
       <c r="P1060" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1060" s="5"/>
       <c r="R1060" s="5"/>
@@ -68134,7 +68134,7 @@
       <c r="A1061" s="4"/>
       <c r="B1061" s="5"/>
       <c r="C1061" s="5" t="s">
-        <v>5313</v>
+        <v>5312</v>
       </c>
       <c r="D1061" s="5"/>
       <c r="E1061" s="5"/>
@@ -68149,7 +68149,7 @@
       <c r="N1061" s="5"/>
       <c r="O1061" s="5"/>
       <c r="P1061" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1061" s="5"/>
       <c r="R1061" s="5"/>
@@ -68169,7 +68169,7 @@
       <c r="A1062" s="4"/>
       <c r="B1062" s="5"/>
       <c r="C1062" s="5" t="s">
-        <v>5314</v>
+        <v>5313</v>
       </c>
       <c r="D1062" s="5"/>
       <c r="E1062" s="5"/>
@@ -68184,7 +68184,7 @@
       <c r="N1062" s="5"/>
       <c r="O1062" s="5"/>
       <c r="P1062" s="10" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1062" s="5"/>
       <c r="R1062" s="5"/>
@@ -68202,16 +68202,16 @@
     </row>
     <row r="1063" spans="1:29">
       <c r="A1063" s="4" t="s">
+        <v>5314</v>
+      </c>
+      <c r="B1063" s="5" t="s">
         <v>5315</v>
-      </c>
-      <c r="B1063" s="5" t="s">
-        <v>5316</v>
       </c>
       <c r="C1063" s="5" t="s">
         <v>2281</v>
       </c>
       <c r="D1063" s="6" t="s">
-        <v>5317</v>
+        <v>5316</v>
       </c>
       <c r="E1063" s="6">
         <v>28356</v>
@@ -68224,28 +68224,28 @@
       </c>
       <c r="H1063" s="5"/>
       <c r="I1063" s="9" t="s">
+        <v>5317</v>
+      </c>
+      <c r="J1063" s="5" t="s">
         <v>5318</v>
       </c>
-      <c r="J1063" s="5" t="s">
+      <c r="K1063" s="11" t="s">
         <v>5319</v>
       </c>
-      <c r="K1063" s="11" t="s">
+      <c r="L1063" s="11" t="s">
         <v>5320</v>
       </c>
-      <c r="L1063" s="11" t="s">
+      <c r="M1063" s="5" t="s">
         <v>5321</v>
       </c>
-      <c r="M1063" s="5" t="s">
+      <c r="N1063" s="11" t="s">
         <v>5322</v>
       </c>
-      <c r="N1063" s="11" t="s">
+      <c r="O1063" s="5" t="s">
         <v>5323</v>
       </c>
-      <c r="O1063" s="5" t="s">
-        <v>5324</v>
-      </c>
       <c r="P1063" s="5" t="s">
-        <v>5264</v>
+        <v>5263</v>
       </c>
       <c r="Q1063" s="5"/>
       <c r="R1063" s="5"/>

</xml_diff>